<commit_message>
Change representation of missing values in Survey_Data
</commit_message>
<xml_diff>
--- a/data/Survey_Data.xlsx
+++ b/data/Survey_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clarebooth/Desktop/Grad school/Classes/MCB 536/tfcb-homework01/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{50D11119-57DB-3846-8568-9395BD82FEDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3C7E3C-178F-894B-B80F-F60D45188CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1980" yWindow="1400" windowWidth="25120" windowHeight="15580" tabRatio="481" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="19">
   <si>
     <t>NA</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>Date_collected</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -94,7 +97,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -139,9 +142,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,7 +536,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -577,7 +580,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -601,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA1DFA22-3496-494C-8D0F-496702D11058}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="161" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="161" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -643,8 +646,12 @@
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -679,8 +686,12 @@
       <c r="D4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -695,8 +706,12 @@
       <c r="D5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -1149,8 +1164,12 @@
         <v>2</v>
       </c>
       <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+      <c r="E28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
@@ -1223,8 +1242,12 @@
         <v>2</v>
       </c>
       <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
+      <c r="E32" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
@@ -1257,8 +1280,12 @@
         <v>2</v>
       </c>
       <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
+      <c r="E34" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="35" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
@@ -1353,11 +1380,17 @@
       <c r="D39" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
+      <c r="E39" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="40" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" s="2"/>
+      <c r="A40" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="B40" s="4">
         <v>41765</v>
       </c>
@@ -1365,8 +1398,12 @@
         <v>3</v>
       </c>
       <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
+      <c r="E40" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="41" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
@@ -1481,8 +1518,12 @@
       <c r="D46" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E46" s="2"/>
-      <c r="F46" s="1"/>
+      <c r="E46" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="47" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">

</xml_diff>